<commit_message>
Changes made in the process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6880049-A97E-436C-9792-D333DAB9A183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -159,14 +172,26 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>DTOE_NetworkSharePath</t>
+  </si>
+  <si>
+    <t>DTOE_Tableau_ReportExtract</t>
+  </si>
+  <si>
+    <t>DetailReport_SheetName</t>
+  </si>
+  <si>
+    <t>DTOE_CombinedReport_NetworkSharePath</t>
+  </si>
+  <si>
+    <t>detail export</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -177,6 +202,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -188,6 +214,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -208,22 +239,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{C6F355A7-D575-447B-977B-71084C6FF74C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,9 +276,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +316,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,16 +574,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -587,14 +624,14 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +641,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -615,7 +652,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1623,12 +1667,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1709,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1834,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +2826,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="2" width="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2828,9 +2873,26 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Made changes to performer
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6880049-A97E-436C-9792-D333DAB9A183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54895633-7C65-4DC4-8FD7-492A760BF664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35460" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>detail export</t>
+  </si>
+  <si>
+    <t>detail report</t>
+  </si>
+  <si>
+    <t>CombinedReport_SheetName</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -660,7 +666,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Removed hard coded values and updated the Perfomer workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54895633-7C65-4DC4-8FD7-492A760BF664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ABBB00-2583-470B-911C-6FBD4BF183C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35460" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31920" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -191,13 +191,25 @@
   </si>
   <si>
     <t>CombinedReport_SheetName</t>
+  </si>
+  <si>
+    <t>DTOE_Crosswalk_SheetName</t>
+  </si>
+  <si>
+    <t>DTOE_Crosswalk_FilePath</t>
+  </si>
+  <si>
+    <t>DTOE_EmailTemplate</t>
+  </si>
+  <si>
+    <t>DTOE_EmailSubject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -227,6 +239,16 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,7 +271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -263,6 +285,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -674,7 +701,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B8" s="2"/>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2839,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2903,12 +2932,37 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added second SendEmail Process for UseCase2 of the workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ABBB00-2583-470B-911C-6FBD4BF183C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B57EC3-2263-451C-8B95-9334AD5CF91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32265" yWindow="3465" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -203,13 +203,16 @@
   </si>
   <si>
     <t>DTOE_EmailSubject</t>
+  </si>
+  <si>
+    <t>DTOE_EmailTemplate2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -249,6 +252,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -290,6 +298,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2869,7 +2878,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2963,7 +2972,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3959,5 +3975,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made adjustments to SendEmail & SentEmailTemplate2
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B57EC3-2263-451C-8B95-9334AD5CF91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F133D094-7972-4E6C-B2F2-85AB71B67E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32265" yWindow="3465" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -206,13 +206,16 @@
   </si>
   <si>
     <t>DTOE_EmailTemplate2</t>
+  </si>
+  <si>
+    <t>TEST_ DTOE_Crosswalk_FilePath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -257,6 +260,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -279,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -299,6 +307,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,12 +629,12 @@
       <selection activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -673,7 +682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -683,7 +692,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1718,12 +1727,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1760,7 +1769,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1771,7 +1780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1885,7 +1894,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2878,14 +2887,14 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2980,7 +2989,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Edits made to SendEmail & SentEmailTemplate2 to reflect new data requirements
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F133D094-7972-4E6C-B2F2-85AB71B67E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BBBF41-19A8-4FB0-9F34-3A9DA135BC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -209,13 +209,16 @@
   </si>
   <si>
     <t>TEST_ DTOE_Crosswalk_FilePath</t>
+  </si>
+  <si>
+    <t>DTOE_EmailSubject_Leadership</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -265,6 +268,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +316,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,12 +638,12 @@
       <selection activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -682,7 +691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -692,7 +701,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1727,12 +1736,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1769,7 +1778,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +1789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1894,7 +1903,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2887,14 +2896,14 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2997,7 +3006,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updates made to SendEmail & SendEmailTemplate2
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BBBF41-19A8-4FB0-9F34-3A9DA135BC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C1EA5A-D608-4F9F-BA1E-1808E0CBAD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -212,13 +212,16 @@
   </si>
   <si>
     <t>DTOE_EmailSubject_Leadership</t>
+  </si>
+  <si>
+    <t>DTOE_SendTestEmail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -273,6 +276,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -295,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,6 +325,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2896,7 +2905,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3014,7 +3023,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Edits to SendEmail, SendEmailTemplate2 and Process applied to satisfy testing parameters and requirements
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C1EA5A-D608-4F9F-BA1E-1808E0CBAD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099803C0-0FDC-4A8F-A6A7-E570E696208D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>DTOE_SendTestEmail</t>
+  </si>
+  <si>
+    <t>FPPS/DTOE</t>
   </si>
 </sst>
 </file>
@@ -643,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -704,7 +707,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -2904,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2958,6 +2963,9 @@
       <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="6" t="s">
@@ -2966,6 +2974,9 @@
       <c r="B3" s="6" t="s">
         <v>47</v>
       </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
@@ -2974,6 +2985,9 @@
       <c r="B4" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
@@ -2982,6 +2996,9 @@
       <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="9" t="s">
@@ -2990,6 +3007,9 @@
       <c r="B6" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
@@ -2998,6 +3018,9 @@
       <c r="B7" t="s">
         <v>54</v>
       </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="10" t="s">
@@ -3006,6 +3029,9 @@
       <c r="B8" s="10" t="s">
         <v>55</v>
       </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="11" t="s">
@@ -3014,6 +3040,9 @@
       <c r="B9" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="12" t="s">
@@ -3022,6 +3051,9 @@
       <c r="B10" s="12" t="s">
         <v>57</v>
       </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="13" t="s">
@@ -3029,6 +3061,9 @@
       </c>
       <c r="B11" s="13" t="s">
         <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Adjustments made to worfklows for PROD data and UAT
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099803C0-0FDC-4A8F-A6A7-E570E696208D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFD92C2-0EE8-4F79-B42E-AA8025B83563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -218,13 +218,16 @@
   </si>
   <si>
     <t>FPPS/DTOE</t>
+  </si>
+  <si>
+    <t>DTOE_SupportEmail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -284,6 +287,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -329,6 +337,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2909,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3066,7 +3075,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Final adjustments to workflow for targeted PROD UAT Added UseCase3 Email Template for additional requirements
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFD92C2-0EE8-4F79-B42E-AA8025B83563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9C44DF-DE09-4F56-96AD-9F6DDAE528F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23070" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -221,13 +221,19 @@
   </si>
   <si>
     <t>DTOE_SupportEmail</t>
+  </si>
+  <si>
+    <t>DTOE_EmailTemplate3</t>
+  </si>
+  <si>
+    <t>DTOE_EmailSubject_Reminder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -292,6 +298,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -314,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,6 +349,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2919,7 +2932,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3086,8 +3099,28 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Adjusted Process to include Email Tracking counts for both use cases
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9C44DF-DE09-4F56-96AD-9F6DDAE528F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B1E899-A5C0-48A8-87F9-B18D82AA8C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23070" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2610" yWindow="3585" windowWidth="22740" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>DTOE_EmailSubject_Reminder</t>
+  </si>
+  <si>
+    <t>DTOE_EmailTracker</t>
   </si>
 </sst>
 </file>
@@ -2932,7 +2935,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3121,7 +3124,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>